<commit_message>
include some eye candy
</commit_message>
<xml_diff>
--- a/LinpackDP/results_paper.xlsx
+++ b/LinpackDP/results_paper.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e77ee0812acbc54/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archive\github\benchmark\LinpackDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{79754ACB-27F1-4BDD-8712-C1B47E91FE5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2B2C1E83-4FDC-418F-8C90-63D28EC78CF5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B425E741-DB16-43E6-9C8B-9C1F6567DDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14040" yWindow="1905" windowWidth="12855" windowHeight="15135" xr2:uid="{949ED96B-E9F4-4CAF-AEB7-403CDBC47196}"/>
+    <workbookView xWindow="29265" yWindow="1680" windowWidth="15075" windowHeight="13305" activeTab="1" xr2:uid="{949ED96B-E9F4-4CAF-AEB7-403CDBC47196}"/>
   </bookViews>
   <sheets>
     <sheet name="paper" sheetId="1" r:id="rId1"/>
+    <sheet name="2025-05" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Platform</t>
   </si>
@@ -136,6 +137,48 @@
   </si>
   <si>
     <t>ARM Cortex-A53 (v8-A) 32bit</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>FLOPS</t>
+  </si>
+  <si>
+    <t>Jetson Nano A02</t>
+  </si>
+  <si>
+    <t>Tegra X1</t>
+  </si>
+  <si>
+    <t>hp zBook 15 G3</t>
+  </si>
+  <si>
+    <t>i7-6820HQ</t>
+  </si>
+  <si>
+    <t>Xigmatek Gemini</t>
+  </si>
+  <si>
+    <t>i3-10100</t>
+  </si>
+  <si>
+    <t>hp mini 400 G9</t>
+  </si>
+  <si>
+    <t>i7-13700T</t>
+  </si>
+  <si>
+    <t>Cores</t>
+  </si>
+  <si>
+    <t>hp MT 600 G4</t>
+  </si>
+  <si>
+    <t>RX 6600</t>
   </si>
 </sst>
 </file>
@@ -187,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -196,9 +239,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -214,7 +261,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -512,11 +559,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838EE691-E486-41EE-8552-5ACAEE3A2AF9}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -771,4 +818,143 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85728D8B-785C-4593-82AB-CE23013FE2C1}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6">
+        <v>94300</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3">
+        <v>1500</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3848500000</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>3600</v>
+      </c>
+      <c r="D4" s="6">
+        <v>99997800000</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>4038</v>
+      </c>
+      <c r="D5" s="6">
+        <v>132278500000</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6">
+        <v>1840</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>2044</v>
+      </c>
+      <c r="D7" s="6">
+        <v>570000000000</v>
+      </c>
+      <c r="E7">
+        <v>1792</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update images, include clpeak benchmark
</commit_message>
<xml_diff>
--- a/LinpackDP/results_paper.xlsx
+++ b/LinpackDP/results_paper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archive\github\benchmark\LinpackDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B425E741-DB16-43E6-9C8B-9C1F6567DDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181537A4-14FE-472E-BF37-A2389C16C7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29265" yWindow="1680" windowWidth="15075" windowHeight="13305" activeTab="1" xr2:uid="{949ED96B-E9F4-4CAF-AEB7-403CDBC47196}"/>
+    <workbookView xWindow="29175" yWindow="2070" windowWidth="15075" windowHeight="13305" activeTab="1" xr2:uid="{949ED96B-E9F4-4CAF-AEB7-403CDBC47196}"/>
   </bookViews>
   <sheets>
     <sheet name="paper" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Platform</t>
   </si>
@@ -179,13 +179,16 @@
   </si>
   <si>
     <t>RX 6600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://openbenchmarking.org/result/2504309-SAIH-KREIER840 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +212,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -227,10 +238,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -243,8 +255,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -822,10 +836,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85728D8B-785C-4593-82AB-CE23013FE2C1}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +850,7 @@
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>34</v>
       </c>
@@ -853,7 +867,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -870,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -887,7 +901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -904,7 +918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -921,7 +935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -929,14 +943,16 @@
         <v>44</v>
       </c>
       <c r="C6">
-        <v>1840</v>
-      </c>
-      <c r="D6" s="6"/>
+        <v>4826</v>
+      </c>
+      <c r="D6" s="6">
+        <v>235712000000</v>
+      </c>
       <c r="E6">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -953,8 +969,25 @@
         <v>1792</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9">
+        <v>1840</v>
+      </c>
+      <c r="D9" s="6">
+        <v>29037000000</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{713DC1C4-CF62-4E06-9053-F1D93515DEB8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>